<commit_message>
add KIT_ME, RWTH_ROBOTICS, DORTMUND_ROBOTICS, TUM_MSNE(not done yet)
</commit_message>
<xml_diff>
--- a/database/ElectricalEngineering/EE_Programs.xlsx
+++ b/database/ElectricalEngineering/EE_Programs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\database\ElectricalEngineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FCF381-23D7-44E6-A889-DDF03CEA503A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C47B7B-8678-419A-AE0E-FA47BC32AA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6975" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program_choosing" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>Program</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>TUM_MSPE</t>
+  </si>
+  <si>
+    <t>TUM_MSNE</t>
   </si>
 </sst>
 </file>
@@ -369,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -428,9 +431,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B6" xr:uid="{610A300D-EA49-404E-A3AA-32352271D928}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B7" xr:uid="{610A300D-EA49-404E-A3AA-32352271D928}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
MSCE not done yet. Add english MTL. fine tune CS,EE.
</commit_message>
<xml_diff>
--- a/database/ElectricalEngineering/EE_Programs.xlsx
+++ b/database/ElectricalEngineering/EE_Programs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\OneDrive\20110706\TaiGer_Transcript-Program_Comparer\database\ElectricalEngineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C47B7B-8678-419A-AE0E-FA47BC32AA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097FD9E0-D122-4639-9391-2A4171D4AE5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6975" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program_choosing" sheetId="1" r:id="rId1"/>
@@ -375,7 +375,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,7 +412,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>